<commit_message>
March 18 1 update
</commit_message>
<xml_diff>
--- a/Jupyter/simulationID/cim_0315_1240/data/bldg/after_212_53.xlsx
+++ b/Jupyter/simulationID/cim_0315_1240/data/bldg/after_212_53.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10203"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shai/Google Drive/BatYam NY DRIVE/Simulations/March 14 GitHUB/BatYamNY/Jupyter/simulationID/cim_0315_1240/data/bldg/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C158053E-C24F-144C-9A99-845FEF0BF404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="37580" yWindow="-2680" windowWidth="28440" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="13">
   <si>
     <t>appUnits</t>
   </si>
@@ -58,8 +64,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +128,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -168,7 +182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,9 +214,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,6 +266,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,14 +459,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,203 +503,539 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>97</v>
+      </c>
+      <c r="E2">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F2">
+        <v>71.5</v>
+      </c>
       <c r="G2">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H2">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I2">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J2">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K2">
+        <v>727.27260000000001</v>
       </c>
       <c r="L2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>97</v>
+      </c>
+      <c r="E3">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F3">
+        <v>71.5</v>
+      </c>
       <c r="G3">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H3">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I3">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J3">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K3">
+        <v>727.27260000000001</v>
       </c>
       <c r="L3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>97</v>
+      </c>
+      <c r="E4">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F4">
+        <v>71.5</v>
+      </c>
       <c r="G4">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H4">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I4">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J4">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K4">
+        <v>727.27260000000001</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>97</v>
+      </c>
+      <c r="E5">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F5">
+        <v>71.5</v>
+      </c>
       <c r="G5">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H5">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I5">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J5">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K5">
+        <v>727.27260000000001</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>97</v>
+      </c>
+      <c r="E6">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F6">
+        <v>71.5</v>
+      </c>
       <c r="G6">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H6">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I6">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J6">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K6">
+        <v>727.27260000000001</v>
       </c>
       <c r="L6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>97</v>
+      </c>
+      <c r="E7">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F7">
+        <v>71.5</v>
+      </c>
       <c r="G7">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H7">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I7">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J7">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K7">
+        <v>727.27260000000001</v>
       </c>
       <c r="L7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>97</v>
+      </c>
+      <c r="E8">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F8">
+        <v>71.5</v>
+      </c>
       <c r="G8">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H8">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I8">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J8">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K8">
+        <v>727.27260000000001</v>
       </c>
       <c r="L8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>97</v>
+      </c>
+      <c r="E9">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F9">
+        <v>71.5</v>
+      </c>
       <c r="G9">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H9">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I9">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J9">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K9">
+        <v>727.27260000000001</v>
       </c>
       <c r="L9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>97</v>
+      </c>
+      <c r="E10">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F10">
+        <v>71.5</v>
+      </c>
       <c r="G10">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H10">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I10">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J10">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K10">
+        <v>727.27260000000001</v>
       </c>
       <c r="L10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>97</v>
+      </c>
+      <c r="E11">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F11">
+        <v>71.5</v>
+      </c>
       <c r="G11">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H11">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I11">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J11">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K11">
+        <v>727.27260000000001</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>97</v>
+      </c>
+      <c r="E12">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F12">
+        <v>71.5</v>
+      </c>
       <c r="G12">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H12">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I12">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J12">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K12">
+        <v>727.27260000000001</v>
       </c>
       <c r="L12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>97</v>
+      </c>
+      <c r="E13">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F13">
+        <v>71.5</v>
+      </c>
       <c r="G13">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H13">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I13">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J13">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K13">
+        <v>727.27260000000001</v>
       </c>
       <c r="L13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>97</v>
+      </c>
+      <c r="E14">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F14">
+        <v>71.5</v>
+      </c>
       <c r="G14">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H14">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I14">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J14">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K14">
+        <v>727.27260000000001</v>
       </c>
       <c r="L14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>97</v>
+      </c>
+      <c r="E15">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F15">
+        <v>71.5</v>
+      </c>
       <c r="G15">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H15">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I15">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J15">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K15">
+        <v>727.27260000000001</v>
       </c>
       <c r="L15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -661,571 +1049,1507 @@
         <v>97</v>
       </c>
       <c r="E16">
-        <v>29674.12127272727</v>
+        <v>29674.121272727269</v>
       </c>
       <c r="F16">
         <v>71.5</v>
       </c>
       <c r="G16">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
       </c>
       <c r="H16">
-        <v>527.2726</v>
+        <v>527.27260000000001</v>
       </c>
       <c r="I16">
-        <v>2878389.763454545</v>
+        <v>2878389.7634545448</v>
       </c>
       <c r="J16">
-        <v>7662.7726</v>
+        <v>7662.7726000000002</v>
       </c>
       <c r="K16">
-        <v>727.2726</v>
+        <v>727.27260000000001</v>
       </c>
       <c r="L16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>97</v>
+      </c>
+      <c r="E17">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F17">
+        <v>71.5</v>
+      </c>
       <c r="G17">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H17">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I17">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J17">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K17">
+        <v>727.27260000000001</v>
       </c>
       <c r="L17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>97</v>
+      </c>
+      <c r="E18">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F18">
+        <v>71.5</v>
+      </c>
       <c r="G18">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H18">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I18">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J18">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K18">
+        <v>727.27260000000001</v>
       </c>
       <c r="L18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>97</v>
+      </c>
+      <c r="E19">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F19">
+        <v>71.5</v>
+      </c>
       <c r="G19">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H19">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I19">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J19">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K19">
+        <v>727.27260000000001</v>
       </c>
       <c r="L19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>97</v>
+      </c>
+      <c r="E20">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F20">
+        <v>71.5</v>
+      </c>
       <c r="G20">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H20">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I20">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J20">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K20">
+        <v>727.27260000000001</v>
       </c>
       <c r="L20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>97</v>
+      </c>
+      <c r="E21">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F21">
+        <v>71.5</v>
+      </c>
       <c r="G21">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H21">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I21">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J21">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K21">
+        <v>727.27260000000001</v>
       </c>
       <c r="L21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>97</v>
+      </c>
+      <c r="E22">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F22">
+        <v>71.5</v>
+      </c>
       <c r="G22">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H22">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I22">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J22">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K22">
+        <v>727.27260000000001</v>
       </c>
       <c r="L22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>97</v>
+      </c>
+      <c r="E23">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F23">
+        <v>71.5</v>
+      </c>
       <c r="G23">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H23">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I23">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J23">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K23">
+        <v>727.27260000000001</v>
       </c>
       <c r="L23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>97</v>
+      </c>
+      <c r="E24">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F24">
+        <v>71.5</v>
+      </c>
       <c r="G24">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H24">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I24">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J24">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K24">
+        <v>727.27260000000001</v>
       </c>
       <c r="L24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>97</v>
+      </c>
+      <c r="E25">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F25">
+        <v>71.5</v>
+      </c>
       <c r="G25">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H25">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I25">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J25">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K25">
+        <v>727.27260000000001</v>
       </c>
       <c r="L25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>97</v>
+      </c>
+      <c r="E26">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F26">
+        <v>71.5</v>
+      </c>
       <c r="G26">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H26">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I26">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J26">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K26">
+        <v>727.27260000000001</v>
       </c>
       <c r="L26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>97</v>
+      </c>
+      <c r="E27">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F27">
+        <v>71.5</v>
+      </c>
       <c r="G27">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H27">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I27">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J27">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K27">
+        <v>727.27260000000001</v>
       </c>
       <c r="L27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>97</v>
+      </c>
+      <c r="E28">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F28">
+        <v>71.5</v>
+      </c>
       <c r="G28">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H28">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I28">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J28">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K28">
+        <v>727.27260000000001</v>
       </c>
       <c r="L28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
         <v>27</v>
       </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>97</v>
+      </c>
+      <c r="E29">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F29">
+        <v>71.5</v>
+      </c>
       <c r="G29">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H29">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I29">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J29">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K29">
+        <v>727.27260000000001</v>
       </c>
       <c r="L29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>97</v>
+      </c>
+      <c r="E30">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F30">
+        <v>71.5</v>
+      </c>
       <c r="G30">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H30">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I30">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J30">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K30">
+        <v>727.27260000000001</v>
       </c>
       <c r="L30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
         <v>29</v>
       </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>97</v>
+      </c>
+      <c r="E31">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F31">
+        <v>71.5</v>
+      </c>
       <c r="G31">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H31">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I31">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J31">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K31">
+        <v>727.27260000000001</v>
       </c>
       <c r="L31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
         <v>30</v>
       </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>97</v>
+      </c>
+      <c r="E32">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F32">
+        <v>71.5</v>
+      </c>
       <c r="G32">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H32">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I32">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J32">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K32">
+        <v>727.27260000000001</v>
       </c>
       <c r="L32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
         <v>31</v>
       </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>97</v>
+      </c>
+      <c r="E33">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F33">
+        <v>71.5</v>
+      </c>
       <c r="G33">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H33">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I33">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J33">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K33">
+        <v>727.27260000000001</v>
       </c>
       <c r="L33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>97</v>
+      </c>
+      <c r="E34">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F34">
+        <v>71.5</v>
+      </c>
       <c r="G34">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H34">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I34">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J34">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K34">
+        <v>727.27260000000001</v>
       </c>
       <c r="L34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
         <v>33</v>
       </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>97</v>
+      </c>
+      <c r="E35">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F35">
+        <v>71.5</v>
+      </c>
       <c r="G35">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H35">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I35">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J35">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K35">
+        <v>727.27260000000001</v>
       </c>
       <c r="L35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
         <v>34</v>
       </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>97</v>
+      </c>
+      <c r="E36">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F36">
+        <v>71.5</v>
+      </c>
       <c r="G36">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H36">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I36">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J36">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K36">
+        <v>727.27260000000001</v>
       </c>
       <c r="L36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
         <v>35</v>
       </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>97</v>
+      </c>
+      <c r="E37">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F37">
+        <v>71.5</v>
+      </c>
       <c r="G37">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H37">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I37">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J37">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K37">
+        <v>727.27260000000001</v>
       </c>
       <c r="L37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
         <v>36</v>
       </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38">
+        <v>97</v>
+      </c>
+      <c r="E38">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F38">
+        <v>71.5</v>
+      </c>
       <c r="G38">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H38">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I38">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J38">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K38">
+        <v>727.27260000000001</v>
       </c>
       <c r="L38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
         <v>37</v>
       </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>97</v>
+      </c>
+      <c r="E39">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F39">
+        <v>71.5</v>
+      </c>
       <c r="G39">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H39">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I39">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J39">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K39">
+        <v>727.27260000000001</v>
       </c>
       <c r="L39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
         <v>38</v>
       </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>97</v>
+      </c>
+      <c r="E40">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F40">
+        <v>71.5</v>
+      </c>
       <c r="G40">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H40">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I40">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J40">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K40">
+        <v>727.27260000000001</v>
       </c>
       <c r="L40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41">
+        <v>97</v>
+      </c>
+      <c r="E41">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F41">
+        <v>71.5</v>
+      </c>
       <c r="G41">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H41">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I41">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J41">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K41">
+        <v>727.27260000000001</v>
       </c>
       <c r="L41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42">
+        <v>97</v>
+      </c>
+      <c r="E42">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F42">
+        <v>71.5</v>
+      </c>
       <c r="G42">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H42">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I42">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J42">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K42">
+        <v>727.27260000000001</v>
       </c>
       <c r="L42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
         <v>41</v>
       </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43">
+        <v>97</v>
+      </c>
+      <c r="E43">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F43">
+        <v>71.5</v>
+      </c>
       <c r="G43">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H43">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I43">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J43">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K43">
+        <v>727.27260000000001</v>
       </c>
       <c r="L43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
         <v>42</v>
       </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44">
+        <v>97</v>
+      </c>
+      <c r="E44">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F44">
+        <v>71.5</v>
+      </c>
       <c r="G44">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H44">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I44">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J44">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K44">
+        <v>727.27260000000001</v>
       </c>
       <c r="L44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
         <v>43</v>
       </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45">
+        <v>97</v>
+      </c>
+      <c r="E45">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F45">
+        <v>71.5</v>
+      </c>
       <c r="G45">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H45">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I45">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J45">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K45">
+        <v>727.27260000000001</v>
       </c>
       <c r="L45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
         <v>44</v>
       </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46">
+        <v>97</v>
+      </c>
+      <c r="E46">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F46">
+        <v>71.5</v>
+      </c>
       <c r="G46">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H46">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I46">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J46">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K46">
+        <v>727.27260000000001</v>
       </c>
       <c r="L46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47">
+        <v>97</v>
+      </c>
+      <c r="E47">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F47">
+        <v>71.5</v>
+      </c>
       <c r="G47">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H47">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I47">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J47">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K47">
+        <v>727.27260000000001</v>
       </c>
       <c r="L47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
         <v>46</v>
       </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48">
+        <v>97</v>
+      </c>
+      <c r="E48">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F48">
+        <v>71.5</v>
+      </c>
       <c r="G48">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H48">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I48">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J48">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K48">
+        <v>727.27260000000001</v>
       </c>
       <c r="L48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
         <v>47</v>
       </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49">
+        <v>97</v>
+      </c>
+      <c r="E49">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F49">
+        <v>71.5</v>
+      </c>
       <c r="G49">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H49">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I49">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J49">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K49">
+        <v>727.27260000000001</v>
       </c>
       <c r="L49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
         <v>48</v>
       </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50">
+        <v>97</v>
+      </c>
+      <c r="E50">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F50">
+        <v>71.5</v>
+      </c>
       <c r="G50">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H50">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I50">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J50">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K50">
+        <v>727.27260000000001</v>
       </c>
       <c r="L50" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
         <v>49</v>
       </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>97</v>
+      </c>
+      <c r="E51">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F51">
+        <v>71.5</v>
+      </c>
       <c r="G51">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H51">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I51">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J51">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K51">
+        <v>727.27260000000001</v>
       </c>
       <c r="L51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52">
         <v>50</v>
       </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <v>97</v>
+      </c>
+      <c r="E52">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F52">
+        <v>71.5</v>
+      </c>
       <c r="G52">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H52">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I52">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J52">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K52">
+        <v>727.27260000000001</v>
       </c>
       <c r="L52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53">
         <v>51</v>
       </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53">
+        <v>97</v>
+      </c>
+      <c r="E53">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F53">
+        <v>71.5</v>
+      </c>
       <c r="G53">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H53">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I53">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J53">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K53">
+        <v>727.27260000000001</v>
       </c>
       <c r="L53" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54">
         <v>52</v>
       </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54">
+        <v>97</v>
+      </c>
+      <c r="E54">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F54">
+        <v>71.5</v>
+      </c>
       <c r="G54">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H54">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I54">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J54">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K54">
+        <v>727.27260000000001</v>
       </c>
       <c r="L54" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55">
         <v>53</v>
       </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55">
+        <v>97</v>
+      </c>
+      <c r="E55">
+        <v>29674.121272727269</v>
+      </c>
+      <c r="F55">
+        <v>71.5</v>
+      </c>
       <c r="G55">
-        <v>5.4358</v>
+        <v>5.4358000000000004</v>
+      </c>
+      <c r="H55">
+        <v>527.27260000000001</v>
+      </c>
+      <c r="I55">
+        <v>2878389.7634545448</v>
+      </c>
+      <c r="J55">
+        <v>7662.7726000000002</v>
+      </c>
+      <c r="K55">
+        <v>727.27260000000001</v>
       </c>
       <c r="L55" t="s">
         <v>12</v>

</xml_diff>